<commit_message>
updated templates and requirements
</commit_message>
<xml_diff>
--- a/templates/Game_Library_Template.xlsx
+++ b/templates/Game_Library_Template.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Coding\Python\Scripts\1-Complete-Projects\Game-Library-Tracker\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC009DA-2ACB-4CF6-B467-A3C2AEBD87D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4CC7E2-79EF-4566-AF96-A9D176D6498C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="5490" windowWidth="22935" windowHeight="16815" tabRatio="172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Games!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Games!$A$1:$Z$1</definedName>
     <definedName name="My_Rating">Games!$C:$C</definedName>
     <definedName name="Name">Games!$H:$H</definedName>
   </definedNames>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Date Added</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>App ID</t>
+  </si>
+  <si>
+    <t>User Tags</t>
+  </si>
+  <si>
+    <t>Last Play Time</t>
+  </si>
+  <si>
+    <t>Time Played</t>
   </si>
 </sst>
 </file>
@@ -222,7 +231,107 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -816,11 +925,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,20 +946,23 @@
     <col min="10" max="10" width="11.7109375" style="9" customWidth="1"/>
     <col min="11" max="12" width="20.7109375" style="4" customWidth="1"/>
     <col min="13" max="13" width="31.140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="9" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" style="9" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.140625" style="9" customWidth="1"/>
-    <col min="19" max="19" width="14" style="7" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" style="8" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" style="8" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" style="5" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" style="9" customWidth="1"/>
-    <col min="24" max="447" width="9.140625" style="6" customWidth="1"/>
-    <col min="448" max="16384" width="9.140625" style="6"/>
+    <col min="14" max="14" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" style="9" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" style="9" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.140625" style="9" customWidth="1"/>
+    <col min="20" max="20" width="11" style="9" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" style="9" customWidth="1"/>
+    <col min="22" max="22" width="14" style="7" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" style="8" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" style="8" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="5" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" style="9" customWidth="1"/>
+    <col min="27" max="450" width="9.140625" style="6" customWidth="1"/>
+    <col min="451" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -890,79 +1002,84 @@
       <c r="M1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W1" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W1">
-      <sortCondition ref="Q1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:Z1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="30" priority="40" operator="containsText" text="GOG">
+    <cfRule type="containsText" dxfId="40" priority="45" operator="containsText" text="GOG">
       <formula>NOT(ISERROR(SEARCH("GOG",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="MS">
+    <cfRule type="containsText" dxfId="39" priority="48" operator="containsText" text="MS">
       <formula>NOT(ISERROR(SEARCH("MS",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="51" operator="containsText" text="Not Enough Data">
+    <cfRule type="containsText" dxfId="38" priority="56" operator="containsText" text="Not Enough Data">
       <formula>NOT(ISERROR(SEARCH("Not Enough Data",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="63" operator="containsText" text="PS5">
+    <cfRule type="containsText" dxfId="37" priority="68" operator="containsText" text="PS5">
       <formula>NOT(ISERROR(SEARCH("PS5",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="64" operator="containsText" text="Uplay">
+    <cfRule type="containsText" dxfId="36" priority="69" operator="containsText" text="Uplay">
       <formula>NOT(ISERROR(SEARCH("Uplay",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="65" operator="containsText" text="Switch">
+    <cfRule type="containsText" dxfId="35" priority="70" operator="containsText" text="Switch">
       <formula>NOT(ISERROR(SEARCH("Switch",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="66" operator="containsText" text="PS4">
+    <cfRule type="containsText" dxfId="34" priority="71" operator="containsText" text="PS4">
       <formula>NOT(ISERROR(SEARCH("PS4",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="67" operator="containsText" text="Steam">
+    <cfRule type="containsText" dxfId="33" priority="72" operator="containsText" text="Steam">
       <formula>NOT(ISERROR(SEARCH("Steam",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="containsText" dxfId="22" priority="10" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",O1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="11" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",O1)))</formula>
+  <conditionalFormatting sqref="P1:P1048576">
+    <cfRule type="containsText" dxfId="32" priority="15" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",P1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="16" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -974,42 +1091,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="20" priority="8" operator="containsText" text="Must Play">
+    <cfRule type="containsText" dxfId="30" priority="13" operator="containsText" text="Must Play">
       <formula>NOT(ISERROR(SEARCH("Must Play",I1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="43" operator="equal">
       <formula>"Endless"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="49" operator="containsText" text="Removed">
+    <cfRule type="containsText" dxfId="28" priority="54" operator="containsText" text="Removed">
       <formula>NOT(ISERROR(SEARCH("Removed",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="53" operator="containsText" text="Software">
+    <cfRule type="containsText" dxfId="27" priority="58" operator="containsText" text="Software">
       <formula>NOT(ISERROR(SEARCH("Software",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="56" operator="containsText" text="Waiting">
+    <cfRule type="containsText" dxfId="26" priority="61" operator="containsText" text="Waiting">
       <formula>NOT(ISERROR(SEARCH("Waiting",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="57" operator="containsText" text="Unplayed">
+    <cfRule type="containsText" dxfId="25" priority="62" operator="containsText" text="Unplayed">
       <formula>NOT(ISERROR(SEARCH("Unplayed",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="58" operator="containsText" text="Playing">
+    <cfRule type="containsText" dxfId="24" priority="63" operator="containsText" text="Playing">
       <formula>NOT(ISERROR(SEARCH("Playing",I1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="59" operator="beginsWith" text="Played">
+    <cfRule type="beginsWith" dxfId="23" priority="64" operator="beginsWith" text="Played">
       <formula>LEFT(I1,LEN("Played"))="Played"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="60" operator="containsText" text="Ignore">
+    <cfRule type="containsText" dxfId="22" priority="65" operator="containsText" text="Ignore">
       <formula>NOT(ISERROR(SEARCH("Ignore",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="61" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="21" priority="66" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="62" operator="containsText" text="Quit">
+    <cfRule type="containsText" dxfId="20" priority="67" operator="containsText" text="Quit">
       <formula>NOT(ISERROR(SEARCH("Quit",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T1:U1048576">
-    <cfRule type="dataBar" priority="1271">
+  <conditionalFormatting sqref="W1:X1048576">
+    <cfRule type="dataBar" priority="1276">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="num" val="6000"/>
@@ -1018,43 +1135,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
-    <cfRule type="timePeriod" dxfId="9" priority="1" timePeriod="last7Days">
+    <cfRule type="timePeriod" dxfId="19" priority="6" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(A1,1)&lt;=6,FLOOR(A1,1)&lt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="8" priority="6" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="18" priority="11" timePeriod="today">
       <formula>FLOOR(A1,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",N1)))</formula>
-    </cfRule>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",O1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R1048576">
+    <cfRule type="top10" dxfId="16" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="top10" dxfId="6" priority="4" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="containsText" dxfId="5" priority="12" operator="containsText" text="Playable">
-      <formula>NOT(ISERROR(SEARCH("Playable",P1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="13" operator="containsText" text="Unsupported">
-      <formula>NOT(ISERROR(SEARCH("Unsupported",P1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="Verified">
-      <formula>NOT(ISERROR(SEARCH("Verified",P1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="44" operator="containsText" text="Unknown">
-      <formula>NOT(ISERROR(SEARCH("Unknown",P1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S1:S1048576">
-    <cfRule type="top10" dxfId="1" priority="3" percent="1" rank="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R1048576">
-    <cfRule type="aboveAverage" dxfId="0" priority="2"/>
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="Playable">
+      <formula>NOT(ISERROR(SEARCH("Playable",Q1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="Unsupported">
+      <formula>NOT(ISERROR(SEARCH("Unsupported",Q1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="20" operator="containsText" text="Verified">
+      <formula>NOT(ISERROR(SEARCH("Verified",Q1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="49" operator="containsText" text="Unknown">
+      <formula>NOT(ISERROR(SEARCH("Unknown",Q1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1:V1048576">
+    <cfRule type="top10" dxfId="11" priority="8" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:U1048576 S1">
+    <cfRule type="aboveAverage" dxfId="10" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="colorScale" priority="1272">
+    <cfRule type="colorScale" priority="1277">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1065,6 +1182,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="T1">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Playable">
+      <formula>NOT(ISERROR(SEARCH("Playable",T1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Unsupported">
+      <formula>NOT(ISERROR(SEARCH("Unsupported",T1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Verified">
+      <formula>NOT(ISERROR(SEARCH("Verified",T1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Unknown">
+      <formula>NOT(ISERROR(SEARCH("Unknown",T1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1">
+    <cfRule type="aboveAverage" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>